<commit_message>
Decided to go with verbose text.  Test font size on phone.
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\Blindesigners\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2882EB03-F51B-4DC3-9878-33A154D91453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC44346-43D2-4403-8DBC-E85676C8706B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19656" yWindow="1536" windowWidth="15504" windowHeight="21120" xr2:uid="{BE9F42BC-5970-4CE2-8E20-E3337A34CC05}"/>
+    <workbookView xWindow="19656" yWindow="1536" windowWidth="15504" windowHeight="21120" activeTab="2" xr2:uid="{BE9F42BC-5970-4CE2-8E20-E3337A34CC05}"/>
   </bookViews>
   <sheets>
     <sheet name="Card" sheetId="1" r:id="rId1"/>
     <sheet name="Website" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Get Yourself Some Cards!</t>
   </si>
@@ -709,7 +710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E638810B-CA41-4111-9EB3-48F32535F78F}">
   <dimension ref="B1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -797,7 +798,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
@@ -915,4 +916,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A88A212-6528-4258-B47F-98B4D9AC5A3C}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.5546875" customWidth="1"/>
+    <col min="2" max="2" width="56.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="7"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:3" ht="63" x14ac:dyDescent="1.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7"/>
+      <c r="C3" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>